<commit_message>
Actualized checkboadr. Began add puts to HashMaP
</commit_message>
<xml_diff>
--- a/checkboard.xlsx
+++ b/checkboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikodem\materialy studia\5 semestr\GK\LAB-3\Algorithm_encryption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCE8BA6-6330-49CB-90AD-D7BED50F46AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7705C0-A55E-4E41-8E6F-4C7484B30D7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{7C2DFB47-843D-429B-8BC3-48F92CAA7F25}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Q</t>
   </si>
@@ -127,6 +127,114 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>Ń</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>ą</t>
+  </si>
+  <si>
+    <t>ć</t>
+  </si>
+  <si>
+    <t>ł</t>
+  </si>
+  <si>
+    <t>ń</t>
+  </si>
+  <si>
+    <t>ó</t>
+  </si>
+  <si>
+    <t>ż</t>
+  </si>
+  <si>
+    <t>ź</t>
+  </si>
+  <si>
+    <t>ś</t>
+  </si>
+  <si>
+    <t>Ś</t>
   </si>
 </sst>
 </file>
@@ -538,14 +646,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A954A9-7E4C-419B-B2A6-DFB73A14C2D1}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" customWidth="1"/>
     <col min="5" max="5" width="3.7109375" customWidth="1"/>
@@ -602,54 +711,46 @@
         <v>2</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -657,34 +758,34 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -692,29 +793,169 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added simple endoding and began decoding
</commit_message>
<xml_diff>
--- a/checkboard.xlsx
+++ b/checkboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikodem\materialy studia\5 semestr\GK\LAB-3\Algorithm_encryption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7705C0-A55E-4E41-8E6F-4C7484B30D7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AE4B8A-BCB6-4827-BD84-7E4329735C37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{7C2DFB47-843D-429B-8BC3-48F92CAA7F25}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Q</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Ś</t>
+  </si>
+  <si>
+    <t>[space]</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +956,9 @@
       <c r="H9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>

</xml_diff>

<commit_message>
working encrypion and decrypion without extra key
</commit_message>
<xml_diff>
--- a/checkboard.xlsx
+++ b/checkboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikodem\materialy studia\5 semestr\GK\LAB-3\Algorithm_encryption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AE4B8A-BCB6-4827-BD84-7E4329735C37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEAD5A7-05FE-4BCF-B841-50EED427388E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{7C2DFB47-843D-429B-8BC3-48F92CAA7F25}"/>
   </bookViews>
@@ -652,7 +652,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
all encoding refactored and working workig
</commit_message>
<xml_diff>
--- a/checkboard.xlsx
+++ b/checkboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikodem\materialy studia\5 semestr\GK\LAB-3\Algorithm_encryption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEAD5A7-05FE-4BCF-B841-50EED427388E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23BB51D-6CCE-41BA-861D-C010CEC29833}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{7C2DFB47-843D-429B-8BC3-48F92CAA7F25}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>Q</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>[space]</t>
+  </si>
+  <si>
+    <t>ę</t>
   </si>
 </sst>
 </file>
@@ -649,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A954A9-7E4C-419B-B2A6-DFB73A14C2D1}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +673,7 @@
     <col min="12" max="12" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -701,9 +704,41 @@
       <c r="K1" s="2">
         <v>9</v>
       </c>
+      <c r="O1" s="2">
+        <v>0</v>
+      </c>
+      <c r="P1" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2">
+        <v>3</v>
+      </c>
+      <c r="S1" s="2">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2">
+        <v>5</v>
+      </c>
+      <c r="U1" s="2">
+        <v>6</v>
+      </c>
+      <c r="V1" s="2">
+        <v>7</v>
+      </c>
+      <c r="W1" s="2">
+        <v>8</v>
+      </c>
+      <c r="X1" s="2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,8 +755,32 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
+      <c r="O2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -755,8 +814,41 @@
       <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N3" s="2">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>5</v>
       </c>
@@ -790,8 +882,41 @@
       <c r="K4" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="N4" s="2">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>8</v>
       </c>
@@ -825,8 +950,41 @@
       <c r="K5" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="N5" s="2">
+        <v>5</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -861,7 +1019,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -896,7 +1054,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>9</v>
       </c>
@@ -931,7 +1089,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -964,5 +1122,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all encoding refactored and working workig v2
</commit_message>
<xml_diff>
--- a/checkboard.xlsx
+++ b/checkboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikodem\materialy studia\5 semestr\GK\LAB-3\Algorithm_encryption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23BB51D-6CCE-41BA-861D-C010CEC29833}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC799EF1-4940-420C-A4CD-49C7919F6F86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{7C2DFB47-843D-429B-8BC3-48F92CAA7F25}"/>
   </bookViews>
@@ -655,7 +655,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="O11" sqref="O11:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
encrypt and decrypt worikin
</commit_message>
<xml_diff>
--- a/checkboard.xlsx
+++ b/checkboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikodem\materialy studia\5 semestr\GK\LAB-3\Algorithm_encryption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC799EF1-4940-420C-A4CD-49C7919F6F86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E4C799-E576-4547-880A-D66F47846EB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{7C2DFB47-843D-429B-8BC3-48F92CAA7F25}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>Q</t>
   </si>
@@ -655,7 +655,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11:R14"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,30 +755,16 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="O2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
-      <c r="U2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1018,6 +1004,35 @@
       <c r="K6" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2">

</xml_diff>

<commit_message>
changed directory of fully working application
</commit_message>
<xml_diff>
--- a/checkboard.xlsx
+++ b/checkboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikodem\materialy studia\5 semestr\GK\LAB-3\Algorithm_encryption\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikodem\materialy studia\5 semestr\POD\LAB-3\Algorithm_encryption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E4C799-E576-4547-880A-D66F47846EB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E2A9A1-534A-45BD-B640-94D80421D7E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{7C2DFB47-843D-429B-8BC3-48F92CAA7F25}"/>
   </bookViews>
@@ -25,103 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Ą</t>
-  </si>
-  <si>
-    <t>Ć</t>
-  </si>
-  <si>
-    <t>Ł</t>
-  </si>
-  <si>
-    <t>Ó</t>
-  </si>
-  <si>
-    <t>Ż</t>
-  </si>
-  <si>
-    <t>Ź</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>.</t>
   </si>
@@ -129,9 +33,6 @@
     <t>,</t>
   </si>
   <si>
-    <t>Ń</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -232,9 +133,6 @@
   </si>
   <si>
     <t>ś</t>
-  </si>
-  <si>
-    <t>Ś</t>
   </si>
   <si>
     <t>[space]</t>
@@ -652,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A954A9-7E4C-419B-B2A6-DFB73A14C2D1}">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +571,7 @@
     <col min="12" max="12" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -704,50 +602,11 @@
       <c r="K1" s="2">
         <v>9</v>
       </c>
-      <c r="O1" s="2">
-        <v>0</v>
-      </c>
-      <c r="P1" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>2</v>
-      </c>
-      <c r="R1" s="2">
-        <v>3</v>
-      </c>
-      <c r="S1" s="2">
-        <v>4</v>
-      </c>
-      <c r="T1" s="2">
-        <v>5</v>
-      </c>
-      <c r="U1" s="2">
-        <v>6</v>
-      </c>
-      <c r="V1" s="2">
-        <v>7</v>
-      </c>
-      <c r="W1" s="2">
-        <v>8</v>
-      </c>
-      <c r="X1" s="2">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -755,385 +614,142 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="2">
-        <v>4</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="2">
-        <v>2</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>8</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="2">
         <v>5</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="2">
-        <v>1</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>